<commit_message>
Filled in excel spreadsheet-subject data
</commit_message>
<xml_diff>
--- a/subject_Analysis.Tables.xlsx
+++ b/subject_Analysis.Tables.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Missouri State University/RESEARCH/2 projects/SPP-Analysis/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="10_ncr:100000_{F0141121-6886-488B-B509-75176B84DCEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{36173C95-DEEE-2B48-9F58-734A8ABF0136}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SOA200, other, ldt" sheetId="2" r:id="rId1"/>
@@ -22,20 +16,20 @@
     <sheet name="SOA1200, other, naming" sheetId="8" r:id="rId7"/>
     <sheet name="SOA1200, first, naming" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2192" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="67">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -228,11 +222,20 @@
   <si>
     <t>model4c.c</t>
   </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>r2m = 0.003042985</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -265,12 +268,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -287,12 +296,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -569,21 +584,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -618,7 +633,7 @@
     <col min="31" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -707,7 +722,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -757,7 +772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -805,7 +820,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -852,7 +867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -896,7 +911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -932,7 +947,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -967,7 +982,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -999,7 +1014,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1032,7 +1047,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -1064,7 +1079,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -1093,7 +1108,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -1125,7 +1140,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -1157,7 +1172,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -1186,7 +1201,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -1216,7 +1231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -1245,7 +1260,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -1271,7 +1286,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -1292,7 +1307,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -1312,7 +1327,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -1329,7 +1344,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -1349,7 +1364,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -1369,7 +1384,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -1386,7 +1401,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -1404,7 +1419,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -1421,7 +1436,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -1435,7 +1450,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -1447,7 +1462,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -1458,7 +1473,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -1466,7 +1481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -1477,7 +1492,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -1488,7 +1503,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -1496,7 +1511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -1505,7 +1520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -1513,25 +1528,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -1566,7 +1586,7 @@
     <col min="31" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1655,7 +1675,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1705,7 +1725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -1753,7 +1773,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1800,7 +1820,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1844,7 +1864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1880,7 +1900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1915,7 +1935,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1947,7 +1967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1980,7 +2000,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -2012,7 +2032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -2041,7 +2061,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -2073,7 +2093,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -2105,7 +2125,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -2134,7 +2154,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -2164,7 +2184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -2193,7 +2213,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -2219,7 +2239,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -2240,7 +2260,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -2260,7 +2280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -2277,7 +2297,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -2297,7 +2317,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -2317,7 +2337,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -2334,7 +2354,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -2352,7 +2372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -2369,7 +2389,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -2383,7 +2403,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -2395,7 +2415,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -2406,7 +2426,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -2414,7 +2434,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -2425,7 +2445,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -2436,7 +2456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -2444,7 +2464,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -2453,7 +2473,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -2461,7 +2481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
@@ -2469,18 +2489,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView zoomScale="157" zoomScaleNormal="251" workbookViewId="0">
+    <sheetView zoomScale="157" zoomScaleNormal="251" zoomScalePageLayoutView="251" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -2515,7 +2540,7 @@
     <col min="31" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2604,7 +2629,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -2654,7 +2679,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2702,7 +2727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -2749,7 +2774,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -2793,7 +2818,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -2829,7 +2854,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -2864,7 +2889,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -2896,7 +2921,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -2929,7 +2954,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -2961,7 +2986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -2990,7 +3015,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -3022,7 +3047,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -3054,7 +3079,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -3083,7 +3108,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -3113,7 +3138,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -3142,7 +3167,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -3168,7 +3193,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -3189,7 +3214,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -3209,7 +3234,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -3226,7 +3251,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -3246,7 +3271,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -3266,7 +3291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -3283,7 +3308,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -3301,7 +3326,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -3318,7 +3343,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -3332,7 +3357,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -3344,7 +3369,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -3355,7 +3380,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -3363,7 +3388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -3374,7 +3399,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -3385,7 +3410,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -3393,7 +3418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -3402,7 +3427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -3410,26 +3435,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y27" sqref="Y27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -3464,7 +3494,7 @@
     <col min="31" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -3553,10 +3583,25 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B2" s="1">
+        <v>2.6472919999999999E-3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
@@ -3603,10 +3648,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B3" s="1">
+        <v>2.6646769999999998E-3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="1" t="s">
         <v>13</v>
@@ -3651,13 +3711,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B4" s="1">
+        <v>2.7021950000000001E-3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="Q4" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="R4" s="1" t="s">
         <v>13</v>
       </c>
@@ -3698,10 +3776,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B5" s="1">
+        <v>2.7117830000000002E-3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="R5" s="1" t="s">
         <v>13</v>
       </c>
@@ -3742,14 +3835,37 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="2"/>
+      <c r="B6" s="1">
+        <v>2.8662200000000001E-3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="Q6" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="V6" s="1" t="s">
         <v>13</v>
       </c>
@@ -3778,81 +3894,104 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:30" s="3" customFormat="1">
+      <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="P7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" s="3" customFormat="1">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="V8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="V8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P9" s="2"/>
+      <c r="B9" s="1">
+        <v>2.898865E-3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="Q9" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="W9" s="1" t="s">
         <v>13</v>
       </c>
@@ -3878,16 +4017,40 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="B10" s="1">
+        <v>2.9975639999999999E-3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="Q10" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="V10" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="W10" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="X10" s="1" t="s">
         <v>13</v>
       </c>
@@ -3910,13 +4073,37 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B11" s="1">
+        <v>3.0021829999999998E-3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="Q11" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="X11" s="1" t="s">
         <v>13</v>
       </c>
@@ -3939,195 +4126,221 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:30" s="3" customFormat="1">
+      <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="P12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" s="3" customFormat="1">
+      <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="P13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD13" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" s="3" customFormat="1">
+      <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="P14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD14" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" s="3" customFormat="1">
+      <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P15" s="2"/>
-      <c r="W15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="P15" s="4"/>
+      <c r="W15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" s="3" customFormat="1">
+      <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="V16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="V16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD16" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" s="3" customFormat="1">
+      <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="X17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD17" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="X17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD17" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P18" s="2"/>
+      <c r="B18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="Q18" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="W18" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="Y18" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="AB18" s="1" t="s">
         <v>13</v>
       </c>
@@ -4138,246 +4351,274 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:30" s="3" customFormat="1">
+      <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="Q19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD19" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" s="3" customFormat="1">
+      <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="Q20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD20" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="Q20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD20" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" s="3" customFormat="1">
+      <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="P21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD21" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="P21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="W21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD21" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" s="3" customFormat="1">
+      <c r="A22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD22" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="P22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD22" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" s="3" customFormat="1">
+      <c r="A23" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="P23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD23" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="P23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD23" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" s="3" customFormat="1">
+      <c r="A24" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="P24" s="2"/>
-      <c r="W24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD24" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="P24" s="4"/>
+      <c r="W24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD24" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" s="3" customFormat="1">
+      <c r="A25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="V25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD25" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="V25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD25" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" s="3" customFormat="1">
+      <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AB26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD26" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AB26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD26" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P27" s="2"/>
+      <c r="B27" s="1">
+        <v>3.2086630000000001E-3</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="Q27" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="W27" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="Y27" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" s="3" customFormat="1">
+      <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="Q28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V28" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="Q28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" s="3" customFormat="1">
+      <c r="A29" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="Q29" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="Q29" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" s="3" customFormat="1">
+      <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="P30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W30" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="P30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="W30" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" s="3" customFormat="1">
+      <c r="A31" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V31" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="P31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V31" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" s="3" customFormat="1">
+      <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P32" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="P32" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" s="3" customFormat="1">
+      <c r="A33" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P33" s="2"/>
-      <c r="W33" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="P33" s="4"/>
+      <c r="W33" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" s="3" customFormat="1">
+      <c r="A34" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="V34" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="V34" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" s="3" customFormat="1">
+      <c r="A35" s="3" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -4412,7 +4653,7 @@
     <col min="31" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -4501,7 +4742,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -4551,7 +4792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -4599,7 +4840,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -4646,7 +4887,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -4690,7 +4931,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -4726,7 +4967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -4761,7 +5002,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -4793,7 +5034,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -4826,7 +5067,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -4858,7 +5099,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -4887,7 +5128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -4919,7 +5160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -4951,7 +5192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -4980,7 +5221,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -5010,7 +5251,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -5039,7 +5280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -5065,7 +5306,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -5086,7 +5327,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -5106,7 +5347,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -5123,7 +5364,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -5143,7 +5384,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -5163,7 +5404,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -5180,7 +5421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -5198,7 +5439,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -5215,7 +5456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -5229,7 +5470,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -5241,7 +5482,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -5252,7 +5493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -5260,7 +5501,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -5271,7 +5512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -5282,7 +5523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -5290,7 +5531,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -5299,7 +5540,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -5307,25 +5548,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -5360,7 +5606,7 @@
     <col min="31" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -5449,7 +5695,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -5499,7 +5745,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -5547,7 +5793,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -5594,7 +5840,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -5638,7 +5884,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -5674,7 +5920,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -5709,7 +5955,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -5741,7 +5987,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -5774,7 +6020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -5806,7 +6052,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -5835,7 +6081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -5867,7 +6113,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -5899,7 +6145,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -5928,7 +6174,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -5958,7 +6204,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -5987,7 +6233,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -6013,7 +6259,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -6034,7 +6280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -6054,7 +6300,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -6071,7 +6317,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -6091,7 +6337,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -6111,7 +6357,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -6128,7 +6374,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -6146,7 +6392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -6163,7 +6409,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -6177,7 +6423,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -6189,7 +6435,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -6200,7 +6446,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -6208,7 +6454,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -6219,7 +6465,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -6230,7 +6476,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -6238,7 +6484,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -6247,7 +6493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -6255,18 +6501,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6274,7 +6525,7 @@
       <selection pane="topRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -6309,7 +6560,7 @@
     <col min="31" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -6398,7 +6649,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -6448,7 +6699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -6496,7 +6747,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -6543,7 +6794,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -6587,7 +6838,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -6623,7 +6874,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -6658,7 +6909,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -6690,7 +6941,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -6723,7 +6974,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -6755,7 +7006,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -6784,7 +7035,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -6816,7 +7067,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -6848,7 +7099,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -6877,7 +7128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -6907,7 +7158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -6936,7 +7187,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -6962,7 +7213,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -6983,7 +7234,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -7003,7 +7254,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -7020,7 +7271,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -7040,7 +7291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -7060,7 +7311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -7077,7 +7328,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -7095,7 +7346,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -7112,7 +7363,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -7126,7 +7377,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -7138,7 +7389,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -7149,7 +7400,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -7157,7 +7408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -7168,7 +7419,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -7179,7 +7430,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -7187,7 +7438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -7196,7 +7447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -7204,25 +7455,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -7257,7 +7513,7 @@
     <col min="31" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -7346,7 +7602,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -7396,7 +7652,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -7444,7 +7700,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -7491,7 +7747,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -7535,7 +7791,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -7571,7 +7827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -7606,7 +7862,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -7638,7 +7894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -7671,7 +7927,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -7703,7 +7959,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -7732,7 +7988,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -7764,7 +8020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -7796,7 +8052,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -7825,7 +8081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -7855,7 +8111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -7884,7 +8140,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -7910,7 +8166,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -7931,7 +8187,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -7951,7 +8207,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -7968,7 +8224,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -7988,7 +8244,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -8008,7 +8264,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -8025,7 +8281,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -8043,7 +8299,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -8060,7 +8316,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -8074,7 +8330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -8086,7 +8342,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -8097,7 +8353,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -8105,7 +8361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -8116,7 +8372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -8127,7 +8383,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -8135,7 +8391,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -8144,7 +8400,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -8152,12 +8408,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished MLM and added to table
</commit_message>
<xml_diff>
--- a/subject_Analysis.Tables.xlsx
+++ b/subject_Analysis.Tables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KDValentine/Documents/GitHub/SPP-Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac924\Documents\GitHub\SPP-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6015DFBB-5A42-4B19-B841-F3B34CF2D630}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16860" windowHeight="14420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="16860" windowHeight="14415" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOA200, other, ldt" sheetId="2" r:id="rId1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2388" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="67">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -240,7 +241,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -273,7 +274,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,6 +284,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,7 +308,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -313,6 +320,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -596,50 +609,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AC27" sqref="AC27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="1"/>
+    <col min="29" max="29" width="4.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -728,7 +741,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -793,7 +806,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -858,7 +871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -920,7 +933,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -976,7 +989,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1026,7 +1039,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -1061,7 +1074,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -1093,7 +1106,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1140,7 +1153,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -1190,7 +1203,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -1234,7 +1247,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
@@ -1266,7 +1279,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -1298,7 +1311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1327,7 +1340,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -1357,7 +1370,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -1386,7 +1399,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -1412,7 +1425,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -1453,7 +1466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
@@ -1473,7 +1486,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
@@ -1490,7 +1503,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
@@ -1510,7 +1523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>51</v>
       </c>
@@ -1530,7 +1543,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>50</v>
       </c>
@@ -1547,7 +1560,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>52</v>
       </c>
@@ -1565,7 +1578,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>53</v>
       </c>
@@ -1582,7 +1595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
@@ -1596,7 +1609,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -1623,7 +1636,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
@@ -1634,7 +1647,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>57</v>
       </c>
@@ -1642,7 +1655,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
@@ -1653,7 +1666,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>59</v>
       </c>
@@ -1664,7 +1677,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
@@ -1672,7 +1685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>61</v>
       </c>
@@ -1681,7 +1694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>62</v>
       </c>
@@ -1689,7 +1702,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>63</v>
       </c>
@@ -1700,49 +1713,49 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="1"/>
+    <col min="29" max="29" width="4.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1831,10 +1844,22 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B2" s="1">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1881,11 +1906,28 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="2"/>
+      <c r="B3" s="1">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="Q3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1929,13 +1971,28 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B4" s="1">
+        <v>1.4E-3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="Q4" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="R4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1976,10 +2033,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B5" s="1">
+        <v>1.4E-3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="R5" s="1" t="s">
         <v>13</v>
       </c>
@@ -2020,10 +2089,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B6" s="1">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="1" t="s">
         <v>13</v>
@@ -2056,77 +2140,92 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="P7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD7" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="V8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="V8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD8" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="B9" s="1">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="1" t="s">
         <v>13</v>
@@ -2156,10 +2255,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="B10" s="1">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="Q10" s="1" t="s">
         <v>13</v>
       </c>
@@ -2188,10 +2302,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B11" s="1">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="Q11" s="1" t="s">
         <v>13</v>
       </c>
@@ -2217,188 +2346,200 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="P12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="W12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD12" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="P13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD13" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="P14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD14" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="P15" s="2"/>
-      <c r="W15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="P15" s="6"/>
+      <c r="W15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD15" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="V16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="V16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD16" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="X17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD17" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="X17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD17" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="B18" s="1">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P18" s="2"/>
       <c r="Q18" s="1" t="s">
         <v>13</v>
@@ -2416,153 +2557,162 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="Q19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="Q19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD19" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="Q20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD20" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="Q20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD20" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="P21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD21" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="P21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="W21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD21" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD22" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="P22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD22" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="P23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD23" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="P23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD23" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="P24" s="2"/>
-      <c r="W24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD24" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="P24" s="6"/>
+      <c r="W24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD24" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="V25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD25" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="V25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD25" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AB26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD26" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AB26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD26" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="B27" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="1" t="s">
         <v>13</v>
@@ -2570,75 +2720,78 @@
       <c r="W27" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="AC27" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="Q28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V28" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="Q28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V28" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="Q29" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="Q29" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="P30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W30" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="P30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="W30" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="P31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V31" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="P31" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V31" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="P32" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="P32" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="P33" s="2"/>
-      <c r="W33" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="P33" s="6"/>
+      <c r="W33" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="V34" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="V34" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2649,49 +2802,49 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView zoomScale="157" zoomScaleNormal="251" zoomScalePageLayoutView="251" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="1"/>
+    <col min="29" max="29" width="4.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2780,7 +2933,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -2830,7 +2983,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2878,7 +3031,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -2925,7 +3078,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -2969,7 +3122,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -3005,7 +3158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -3040,7 +3193,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -3072,7 +3225,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -3105,7 +3258,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -3137,7 +3290,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -3166,7 +3319,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -3198,7 +3351,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -3230,7 +3383,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -3259,7 +3412,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -3289,7 +3442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -3318,7 +3471,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -3344,7 +3497,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -3365,7 +3518,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -3385,7 +3538,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -3402,7 +3555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -3422,7 +3575,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -3442,7 +3595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -3459,7 +3612,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -3477,7 +3630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -3494,7 +3647,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -3508,7 +3661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -3520,7 +3673,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -3531,7 +3684,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -3539,7 +3692,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -3550,7 +3703,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -3561,7 +3714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -3569,7 +3722,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -3578,7 +3731,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -3586,7 +3739,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
@@ -3598,49 +3751,49 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Y27" sqref="Y27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="1"/>
+    <col min="29" max="29" width="4.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -3729,7 +3882,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -3794,7 +3947,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -3857,7 +4010,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -3922,7 +4075,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -3981,7 +4134,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -4040,7 +4193,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -4075,7 +4228,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -4107,7 +4260,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -4163,7 +4316,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -4219,7 +4372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -4272,7 +4425,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
@@ -4304,7 +4457,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -4336,7 +4489,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -4365,7 +4518,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -4395,7 +4548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -4424,7 +4577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -4450,7 +4603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -4497,7 +4650,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
@@ -4517,7 +4670,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
@@ -4534,7 +4687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
@@ -4554,7 +4707,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>51</v>
       </c>
@@ -4574,7 +4727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>50</v>
       </c>
@@ -4591,7 +4744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>52</v>
       </c>
@@ -4609,7 +4762,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>53</v>
       </c>
@@ -4626,7 +4779,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
@@ -4640,7 +4793,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -4675,7 +4828,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
@@ -4686,7 +4839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>57</v>
       </c>
@@ -4694,7 +4847,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
@@ -4705,7 +4858,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>59</v>
       </c>
@@ -4716,7 +4869,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
@@ -4724,7 +4877,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>61</v>
       </c>
@@ -4733,7 +4886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>62</v>
       </c>
@@ -4741,7 +4894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>63</v>
       </c>
@@ -4752,49 +4905,49 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="1"/>
+    <col min="29" max="29" width="4.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -4883,7 +5036,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -4933,7 +5086,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -4981,7 +5134,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -5028,7 +5181,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -5072,7 +5225,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -5108,7 +5261,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -5143,7 +5296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -5175,7 +5328,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -5208,7 +5361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -5240,7 +5393,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -5269,7 +5422,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -5301,7 +5454,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -5333,7 +5486,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -5362,7 +5515,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -5392,7 +5545,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -5421,7 +5574,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -5447,7 +5600,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -5468,7 +5621,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -5488,7 +5641,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -5505,7 +5658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -5525,7 +5678,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -5545,7 +5698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -5562,7 +5715,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -5580,7 +5733,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -5597,7 +5750,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -5611,7 +5764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -5623,7 +5776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -5634,7 +5787,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -5642,7 +5795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -5653,7 +5806,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -5664,7 +5817,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -5672,7 +5825,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -5681,7 +5834,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -5689,7 +5842,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
@@ -5700,49 +5853,49 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="1"/>
+    <col min="29" max="29" width="4.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -5831,7 +5984,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -5881,7 +6034,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -5929,7 +6082,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -5976,7 +6129,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -6020,7 +6173,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -6056,7 +6209,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -6091,7 +6244,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -6123,7 +6276,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -6156,7 +6309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -6188,7 +6341,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -6217,7 +6370,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -6249,7 +6402,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -6281,7 +6434,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -6310,7 +6463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -6340,7 +6493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -6369,7 +6522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -6395,7 +6548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -6416,7 +6569,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -6436,7 +6589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -6453,7 +6606,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -6473,7 +6626,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -6493,7 +6646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -6510,7 +6663,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -6528,7 +6681,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -6545,7 +6698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -6559,7 +6712,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -6571,7 +6724,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -6582,7 +6735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -6590,7 +6743,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -6601,7 +6754,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -6612,7 +6765,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -6620,7 +6773,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -6629,7 +6782,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -6637,7 +6790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
@@ -6648,7 +6801,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6656,42 +6809,42 @@
       <selection pane="topRight" activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="1"/>
+    <col min="29" max="29" width="4.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -6780,7 +6933,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -6848,7 +7001,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -6914,7 +7067,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -6979,7 +7132,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -7041,7 +7194,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -7095,7 +7248,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -7149,7 +7302,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -7201,7 +7354,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -7252,7 +7405,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -7308,7 +7461,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -7361,7 +7514,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -7413,7 +7566,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -7465,7 +7618,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -7515,7 +7668,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -7565,7 +7718,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -7615,7 +7768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -7663,7 +7816,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -7702,7 +7855,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -7746,7 +7899,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -7788,7 +7941,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -7832,7 +7985,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -7876,7 +8029,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -7918,7 +8071,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -7960,7 +8113,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -8002,7 +8155,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -8042,7 +8195,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -8072,7 +8225,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -8110,7 +8263,7 @@
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -8146,7 +8299,7 @@
       <c r="AC29" s="3"/>
       <c r="AD29" s="3"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -8184,7 +8337,7 @@
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -8222,7 +8375,7 @@
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -8258,7 +8411,7 @@
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -8294,7 +8447,7 @@
       <c r="AC33" s="3"/>
       <c r="AD33" s="3"/>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -8330,7 +8483,7 @@
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
@@ -8370,49 +8523,49 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AD27" sqref="AD27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="1"/>
+    <col min="29" max="29" width="4.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -8501,7 +8654,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -8563,7 +8716,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -8625,7 +8778,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -8684,7 +8837,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -8740,7 +8893,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -8788,7 +8941,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -8829,7 +8982,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -8867,7 +9020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -8915,7 +9068,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -8962,7 +9115,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -9006,7 +9159,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
@@ -9038,7 +9191,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -9070,7 +9223,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -9099,7 +9252,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -9129,7 +9282,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -9158,7 +9311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -9184,7 +9337,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -9220,7 +9373,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
@@ -9240,7 +9393,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
@@ -9257,7 +9410,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
@@ -9277,7 +9430,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>51</v>
       </c>
@@ -9297,7 +9450,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>50</v>
       </c>
@@ -9314,7 +9467,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>52</v>
       </c>
@@ -9332,7 +9485,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>53</v>
       </c>
@@ -9349,7 +9502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
@@ -9363,7 +9516,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -9390,7 +9543,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
@@ -9401,7 +9554,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>57</v>
       </c>
@@ -9409,7 +9562,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
@@ -9420,7 +9573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>59</v>
       </c>
@@ -9431,7 +9584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
@@ -9439,7 +9592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>61</v>
       </c>
@@ -9448,7 +9601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>62</v>
       </c>
@@ -9456,7 +9609,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
apparently hadn't pushed excel sheet
</commit_message>
<xml_diff>
--- a/subject_Analysis.Tables.xlsx
+++ b/subject_Analysis.Tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber Gillenwaters\Documents\GitHub\SPP-Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac924\Documents\GitHub\SPP-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4799FEE4-C18E-43A4-AD63-EF818091348D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E4AD88-B6F5-4117-868B-924C26BB7932}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="25590" windowHeight="15540" tabRatio="500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="25590" windowHeight="15540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOA200, other, ldt" sheetId="2" r:id="rId1"/>
@@ -22,10 +22,15 @@
     <sheet name="SOA1200, other, naming" sheetId="8" r:id="rId7"/>
     <sheet name="SOA1200, first, naming" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -35,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2286" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="66">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -271,7 +276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,6 +286,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,7 +310,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -318,6 +329,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1551,8 +1568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1683,6 +1700,18 @@
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B2" s="1">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1733,7 +1762,24 @@
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="2"/>
+      <c r="B3" s="1">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="Q3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1781,8 +1827,23 @@
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B4" s="1">
+        <v>1.4E-3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P4" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>13</v>
@@ -1828,6 +1889,18 @@
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B5" s="1">
+        <v>1.4E-3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="R5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1872,6 +1945,21 @@
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B6" s="1">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="1" t="s">
         <v>13</v>
@@ -1904,70 +1992,70 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="P7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD7" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="V8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD8" s="1" t="s">
+      <c r="V8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD8" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1975,6 +2063,21 @@
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="B9" s="1">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="1" t="s">
         <v>13</v>
@@ -2008,6 +2111,21 @@
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="B10" s="1">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="Q10" s="1" t="s">
         <v>13</v>
       </c>
@@ -2040,6 +2158,21 @@
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B11" s="1">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="Q11" s="1" t="s">
         <v>13</v>
       </c>
@@ -2065,181 +2198,181 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="P12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="W12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD12" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="P13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD13" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="P14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD14" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="P15" s="2"/>
-      <c r="W15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="P15" s="8"/>
+      <c r="W15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD15" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="V16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="V16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD16" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="X17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD17" s="1" t="s">
+      <c r="X17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD17" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2247,6 +2380,18 @@
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="B18" s="1">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P18" s="2"/>
       <c r="Q18" s="1" t="s">
         <v>13</v>
@@ -2264,146 +2409,146 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="Q19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="Q19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD19" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="Q20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD20" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="Q20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD20" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="P21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD21" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="P21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="W21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD21" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD22" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="P22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD22" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="P23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD23" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="P23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD23" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="P24" s="2"/>
-      <c r="W24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD24" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="P24" s="8"/>
+      <c r="W24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD24" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="V25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD25" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="V25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD25" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="AB26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD26" s="1" t="s">
+      <c r="AB26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD26" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2411,6 +2556,15 @@
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="B27" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="1" t="s">
         <v>13</v>
@@ -2418,75 +2572,78 @@
       <c r="W27" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="AC27" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="Q28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V28" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="Q28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V28" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="Q29" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="Q29" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="P30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W30" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="P30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="W30" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="P31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V31" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="P31" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V31" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="P32" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="P32" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="P33" s="2"/>
-      <c r="W33" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="P33" s="8"/>
+      <c r="W33" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="V34" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="V34" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>63</v>
       </c>
     </row>
@@ -6443,7 +6600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="O27" sqref="O27"/>
     </sheetView>

</xml_diff>

<commit_message>
filled in subject table
</commit_message>
<xml_diff>
--- a/subject_Analysis.Tables.xlsx
+++ b/subject_Analysis.Tables.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/addiew/Documents/SPP-Analysis/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7E3208-5FDC-5B46-A37A-AC726B24FBAC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11680" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SOA200, other, ldt" sheetId="2" r:id="rId1"/>
@@ -22,20 +16,20 @@
     <sheet name="SOA1200, other, naming" sheetId="8" r:id="rId7"/>
     <sheet name="SOA1200, first, naming" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2379" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="66">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -238,7 +232,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -617,21 +611,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -666,7 +660,7 @@
     <col min="31" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -755,7 +749,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -805,7 +799,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -853,7 +847,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -900,7 +894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -944,7 +938,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -980,7 +974,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1015,7 +1009,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1047,7 +1041,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1080,7 +1074,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -1112,7 +1106,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -1141,7 +1135,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -1173,7 +1167,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -1205,7 +1199,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -1234,7 +1228,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -1264,7 +1258,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -1293,7 +1287,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -1319,7 +1313,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -1340,7 +1334,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -1360,7 +1354,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -1377,7 +1371,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -1397,7 +1391,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -1417,7 +1411,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -1434,7 +1428,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -1452,7 +1446,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -1469,7 +1463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -1483,7 +1477,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -1495,7 +1489,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -1506,7 +1500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -1514,7 +1508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -1525,7 +1519,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -1536,7 +1530,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -1544,7 +1538,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -1553,7 +1547,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -1561,25 +1555,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -1614,7 +1613,7 @@
     <col min="31" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1703,7 +1702,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1765,7 +1764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -1830,7 +1829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1892,7 +1891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1948,7 +1947,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1999,7 +1998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" s="7" customFormat="1">
       <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
@@ -2034,7 +2033,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" s="7" customFormat="1">
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
@@ -2066,7 +2065,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -2114,7 +2113,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -2161,7 +2160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -2205,7 +2204,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" s="7" customFormat="1">
       <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
@@ -2237,7 +2236,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" s="7" customFormat="1">
       <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
@@ -2269,7 +2268,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" s="7" customFormat="1">
       <c r="A14" s="7" t="s">
         <v>27</v>
       </c>
@@ -2298,7 +2297,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" s="7" customFormat="1">
       <c r="A15" s="7" t="s">
         <v>43</v>
       </c>
@@ -2328,7 +2327,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" s="7" customFormat="1">
       <c r="A16" s="7" t="s">
         <v>44</v>
       </c>
@@ -2357,7 +2356,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" s="7" customFormat="1">
       <c r="A17" s="7" t="s">
         <v>45</v>
       </c>
@@ -2383,7 +2382,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -2416,7 +2415,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" s="7" customFormat="1">
       <c r="A19" s="7" t="s">
         <v>47</v>
       </c>
@@ -2436,7 +2435,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" s="7" customFormat="1">
       <c r="A20" s="7" t="s">
         <v>49</v>
       </c>
@@ -2453,7 +2452,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" s="7" customFormat="1">
       <c r="A21" s="7" t="s">
         <v>46</v>
       </c>
@@ -2473,7 +2472,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" s="7" customFormat="1">
       <c r="A22" s="7" t="s">
         <v>51</v>
       </c>
@@ -2493,7 +2492,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" s="7" customFormat="1">
       <c r="A23" s="7" t="s">
         <v>50</v>
       </c>
@@ -2510,7 +2509,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" s="7" customFormat="1">
       <c r="A24" s="7" t="s">
         <v>52</v>
       </c>
@@ -2528,7 +2527,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" s="7" customFormat="1">
       <c r="A25" s="7" t="s">
         <v>53</v>
       </c>
@@ -2545,7 +2544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" s="7" customFormat="1">
       <c r="A26" s="7" t="s">
         <v>54</v>
       </c>
@@ -2559,7 +2558,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -2583,7 +2582,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" s="7" customFormat="1">
       <c r="A28" s="7" t="s">
         <v>56</v>
       </c>
@@ -2594,7 +2593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" s="7" customFormat="1">
       <c r="A29" s="7" t="s">
         <v>57</v>
       </c>
@@ -2602,7 +2601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" s="7" customFormat="1">
       <c r="A30" s="7" t="s">
         <v>58</v>
       </c>
@@ -2613,7 +2612,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" s="7" customFormat="1">
       <c r="A31" s="7" t="s">
         <v>59</v>
       </c>
@@ -2624,7 +2623,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" s="7" customFormat="1">
       <c r="A32" s="7" t="s">
         <v>60</v>
       </c>
@@ -2632,7 +2631,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" s="7" customFormat="1">
       <c r="A33" s="7" t="s">
         <v>61</v>
       </c>
@@ -2641,7 +2640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" s="7" customFormat="1">
       <c r="A34" s="7" t="s">
         <v>62</v>
       </c>
@@ -2649,7 +2648,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" s="7" customFormat="1">
       <c r="A35" s="7" t="s">
         <v>63</v>
       </c>
@@ -2657,18 +2656,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView zoomScale="157" zoomScaleNormal="251" workbookViewId="0">
+    <sheetView zoomScale="157" zoomScaleNormal="251" zoomScalePageLayoutView="251" workbookViewId="0">
       <selection activeCell="AE27" sqref="AE27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -2703,7 +2707,7 @@
     <col min="31" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2792,7 +2796,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -2860,7 +2864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2926,7 +2930,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -2991,7 +2995,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -3053,7 +3057,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -3101,7 +3105,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -3136,7 +3140,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -3168,7 +3172,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -3213,7 +3217,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -3257,7 +3261,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -3298,7 +3302,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" s="3" customFormat="1">
       <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
@@ -3330,7 +3334,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -3362,7 +3366,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" s="3" customFormat="1">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -3391,7 +3395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" s="3" customFormat="1">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -3421,7 +3425,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" s="3" customFormat="1">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -3450,7 +3454,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" s="3" customFormat="1">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -3476,7 +3480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -3512,7 +3516,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" s="3" customFormat="1">
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
@@ -3532,7 +3536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" s="3" customFormat="1">
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
@@ -3549,7 +3553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" s="3" customFormat="1">
       <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
@@ -3569,7 +3573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" s="3" customFormat="1">
       <c r="A22" s="3" t="s">
         <v>51</v>
       </c>
@@ -3589,7 +3593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" s="3" customFormat="1">
       <c r="A23" s="3" t="s">
         <v>50</v>
       </c>
@@ -3606,7 +3610,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" s="3" customFormat="1">
       <c r="A24" s="3" t="s">
         <v>52</v>
       </c>
@@ -3624,7 +3628,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" s="3" customFormat="1">
       <c r="A25" s="3" t="s">
         <v>53</v>
       </c>
@@ -3641,7 +3645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" s="3" customFormat="1">
       <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
@@ -3655,7 +3659,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -3682,7 +3686,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" s="3" customFormat="1">
       <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
@@ -3693,7 +3697,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" s="3" customFormat="1">
       <c r="A29" s="3" t="s">
         <v>57</v>
       </c>
@@ -3701,7 +3705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" s="3" customFormat="1">
       <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
@@ -3712,7 +3716,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" s="3" customFormat="1">
       <c r="A31" s="3" t="s">
         <v>59</v>
       </c>
@@ -3723,7 +3727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" s="3" customFormat="1">
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
@@ -3731,7 +3735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" s="3" customFormat="1">
       <c r="A33" s="3" t="s">
         <v>61</v>
       </c>
@@ -3740,7 +3744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" s="3" customFormat="1">
       <c r="A34" s="3" t="s">
         <v>62</v>
       </c>
@@ -3748,26 +3752,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" s="3" customFormat="1">
       <c r="A35" s="3" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -3802,7 +3811,7 @@
     <col min="31" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -3891,10 +3900,25 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B2" s="1">
+        <v>2.6472919999999999E-3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
@@ -3941,10 +3965,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B3" s="1">
+        <v>2.6646769999999998E-3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="1" t="s">
         <v>13</v>
@@ -3989,13 +4028,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B4" s="1">
+        <v>2.7021950000000001E-3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="Q4" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="R4" s="1" t="s">
         <v>13</v>
       </c>
@@ -4036,10 +4093,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B5" s="1">
+        <v>2.7117830000000002E-3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="R5" s="1" t="s">
         <v>13</v>
       </c>
@@ -4080,14 +4152,37 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="2"/>
+      <c r="B6" s="1">
+        <v>2.8662200000000001E-3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="Q6" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="V6" s="1" t="s">
         <v>13</v>
       </c>
@@ -4116,81 +4211,104 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:30" s="9" customFormat="1">
+      <c r="A7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="P7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="X7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD7" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" s="9" customFormat="1">
+      <c r="A8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="V8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="V8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="W8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD8" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P9" s="2"/>
+      <c r="B9" s="1">
+        <v>2.898865E-3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="Q9" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="W9" s="1" t="s">
         <v>13</v>
       </c>
@@ -4216,16 +4334,40 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="B10" s="1">
+        <v>2.9975639999999999E-3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="Q10" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="V10" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="W10" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="X10" s="1" t="s">
         <v>13</v>
       </c>
@@ -4248,13 +4390,37 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B11" s="1">
+        <v>3.0021829999999998E-3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="Q11" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="X11" s="1" t="s">
         <v>13</v>
       </c>
@@ -4277,195 +4443,219 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:30" s="9" customFormat="1">
+      <c r="A12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="P12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="W12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="X12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD12" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" s="9" customFormat="1">
+      <c r="A13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="P13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="X13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD13" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" s="9" customFormat="1">
+      <c r="A14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="P14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="X14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD14" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" s="9" customFormat="1">
+      <c r="A15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="P15" s="2"/>
-      <c r="W15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="P15" s="10"/>
+      <c r="W15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="X15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD15" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" s="9" customFormat="1">
+      <c r="A16" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="V16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="V16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="X16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD16" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" s="9" customFormat="1">
+      <c r="A17" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="X17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD17" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="X17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD17" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="B18" s="1">
+        <v>3.0429849999999998E-3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="P18" s="2"/>
       <c r="Q18" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="W18" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="Y18" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="AB18" s="1" t="s">
         <v>13</v>
       </c>
@@ -4476,246 +4666,274 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:30" s="9" customFormat="1">
+      <c r="A19" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="Q19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="Q19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD19" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" s="9" customFormat="1">
+      <c r="A20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="Q20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD20" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="Q20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD20" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" s="9" customFormat="1">
+      <c r="A21" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD21" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="P21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="W21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD21" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" s="9" customFormat="1">
+      <c r="A22" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD22" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="P22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD22" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" s="9" customFormat="1">
+      <c r="A23" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="P23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD23" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="P23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD23" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" s="9" customFormat="1">
+      <c r="A24" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="P24" s="2"/>
-      <c r="W24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD24" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="P24" s="10"/>
+      <c r="W24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD24" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" s="9" customFormat="1">
+      <c r="A25" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="V25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD25" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="V25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD25" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" s="9" customFormat="1">
+      <c r="A26" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="AB26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD26" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AB26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD26" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P27" s="2"/>
+      <c r="B27" s="1">
+        <v>3.2086630000000001E-3</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="Q27" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="W27" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="Y27" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" s="9" customFormat="1">
+      <c r="A28" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="Q28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V28" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="Q28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V28" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" s="9" customFormat="1">
+      <c r="A29" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="Q29" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="Q29" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" s="9" customFormat="1">
+      <c r="A30" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="P30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W30" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="P30" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="W30" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" s="9" customFormat="1">
+      <c r="A31" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="P31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V31" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="P31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V31" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" s="9" customFormat="1">
+      <c r="A32" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="P32" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="P32" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" s="9" customFormat="1">
+      <c r="A33" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="P33" s="2"/>
-      <c r="W33" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="P33" s="10"/>
+      <c r="W33" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" s="9" customFormat="1">
+      <c r="A34" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="V34" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="V34" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" s="9" customFormat="1">
+      <c r="A35" s="9" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -4750,7 +4968,7 @@
     <col min="31" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -4839,7 +5057,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -4907,7 +5125,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -4973,7 +5191,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -5038,7 +5256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -5100,7 +5318,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -5157,7 +5375,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" s="9" customFormat="1">
       <c r="A7" s="9" t="s">
         <v>21</v>
       </c>
@@ -5192,7 +5410,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" s="9" customFormat="1">
       <c r="A8" s="9" t="s">
         <v>22</v>
       </c>
@@ -5224,7 +5442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -5278,7 +5496,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -5334,7 +5552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -5387,7 +5605,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" s="9" customFormat="1">
       <c r="A12" s="9" t="s">
         <v>41</v>
       </c>
@@ -5419,7 +5637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" s="9" customFormat="1">
       <c r="A13" s="9" t="s">
         <v>42</v>
       </c>
@@ -5451,7 +5669,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" s="9" customFormat="1">
       <c r="A14" s="9" t="s">
         <v>27</v>
       </c>
@@ -5480,7 +5698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" s="9" customFormat="1">
       <c r="A15" s="9" t="s">
         <v>43</v>
       </c>
@@ -5510,7 +5728,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" s="9" customFormat="1">
       <c r="A16" s="9" t="s">
         <v>44</v>
       </c>
@@ -5539,7 +5757,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" s="9" customFormat="1">
       <c r="A17" s="9" t="s">
         <v>45</v>
       </c>
@@ -5565,7 +5783,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -5604,7 +5822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" s="9" customFormat="1">
       <c r="A19" s="9" t="s">
         <v>47</v>
       </c>
@@ -5624,7 +5842,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" s="9" customFormat="1">
       <c r="A20" s="9" t="s">
         <v>49</v>
       </c>
@@ -5641,7 +5859,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" s="9" customFormat="1">
       <c r="A21" s="9" t="s">
         <v>46</v>
       </c>
@@ -5661,7 +5879,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" s="9" customFormat="1">
       <c r="A22" s="9" t="s">
         <v>51</v>
       </c>
@@ -5681,7 +5899,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" s="9" customFormat="1">
       <c r="A23" s="9" t="s">
         <v>50</v>
       </c>
@@ -5698,7 +5916,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" s="9" customFormat="1">
       <c r="A24" s="9" t="s">
         <v>52</v>
       </c>
@@ -5716,7 +5934,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" s="9" customFormat="1">
       <c r="A25" s="9" t="s">
         <v>53</v>
       </c>
@@ -5733,7 +5951,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" s="9" customFormat="1">
       <c r="A26" s="9" t="s">
         <v>54</v>
       </c>
@@ -5747,7 +5965,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -5777,7 +5995,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" s="9" customFormat="1">
       <c r="A28" s="9" t="s">
         <v>56</v>
       </c>
@@ -5788,7 +6006,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" s="9" customFormat="1">
       <c r="A29" s="9" t="s">
         <v>57</v>
       </c>
@@ -5796,7 +6014,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" s="9" customFormat="1">
       <c r="A30" s="9" t="s">
         <v>58</v>
       </c>
@@ -5807,7 +6025,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" s="9" customFormat="1">
       <c r="A31" s="9" t="s">
         <v>59</v>
       </c>
@@ -5818,7 +6036,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" s="9" customFormat="1">
       <c r="A32" s="9" t="s">
         <v>60</v>
       </c>
@@ -5826,7 +6044,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" s="9" customFormat="1">
       <c r="A33" s="9" t="s">
         <v>61</v>
       </c>
@@ -5835,7 +6053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" s="9" customFormat="1">
       <c r="A34" s="9" t="s">
         <v>62</v>
       </c>
@@ -5843,25 +6061,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" s="9" customFormat="1">
       <c r="A35" s="9" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -5896,7 +6119,7 @@
     <col min="31" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -5985,7 +6208,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -6035,7 +6258,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -6083,7 +6306,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -6130,7 +6353,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -6174,7 +6397,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -6210,7 +6433,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -6245,7 +6468,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -6277,7 +6500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -6310,7 +6533,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -6342,7 +6565,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -6371,7 +6594,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -6403,7 +6626,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -6435,7 +6658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -6464,7 +6687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -6494,7 +6717,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -6523,7 +6746,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -6549,7 +6772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -6570,7 +6793,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -6590,7 +6813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -6607,7 +6830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -6627,7 +6850,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -6647,7 +6870,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -6664,7 +6887,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -6682,7 +6905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -6699,7 +6922,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -6713,7 +6936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -6725,7 +6948,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -6736,7 +6959,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -6744,7 +6967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -6755,7 +6978,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -6766,7 +6989,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -6774,7 +6997,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -6783,7 +7006,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -6791,18 +7014,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6810,7 +7038,7 @@
       <selection pane="topRight" activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="5" customWidth="1"/>
@@ -6845,7 +7073,7 @@
     <col min="31" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="5" t="s">
         <v>23</v>
       </c>
@@ -6934,7 +7162,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -7002,7 +7230,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -7068,7 +7296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -7133,7 +7361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -7195,7 +7423,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -7249,7 +7477,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -7284,7 +7512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -7316,7 +7544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -7367,7 +7595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -7423,7 +7651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -7476,7 +7704,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -7508,7 +7736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -7540,7 +7768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -7569,7 +7797,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -7599,7 +7827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -7628,7 +7856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -7654,7 +7882,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -7693,7 +7921,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -7713,7 +7941,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -7730,7 +7958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -7750,7 +7978,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -7770,7 +7998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -7787,7 +8015,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -7805,7 +8033,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -7822,7 +8050,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -7836,7 +8064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -7866,7 +8094,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -7877,7 +8105,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -7885,7 +8113,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -7896,7 +8124,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -7907,7 +8135,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -7915,7 +8143,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -7924,7 +8152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -7932,26 +8160,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -7986,7 +8219,7 @@
     <col min="31" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -8075,7 +8308,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -8125,7 +8358,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -8173,7 +8406,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -8220,7 +8453,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -8264,7 +8497,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -8300,7 +8533,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -8335,7 +8568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -8367,7 +8600,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -8400,7 +8633,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -8432,7 +8665,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -8461,7 +8694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -8493,7 +8726,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -8525,7 +8758,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -8554,7 +8787,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -8584,7 +8817,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -8613,7 +8846,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -8639,7 +8872,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -8660,7 +8893,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -8680,7 +8913,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -8697,7 +8930,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -8717,7 +8950,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -8737,7 +8970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -8754,7 +8987,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -8772,7 +9005,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -8789,7 +9022,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -8803,7 +9036,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -8815,7 +9048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -8826,7 +9059,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -8834,7 +9067,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -8845,7 +9078,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -8856,7 +9089,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -8864,7 +9097,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -8873,7 +9106,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -8881,12 +9114,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>